<commit_message>
add examples to FamilyMemberHistory, and cleanup narrative.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-FM-adopted.xlsx
+++ b/docs/StructureDefinition-FM-adopted.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/FM-adopted</t>
+    <t>https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/FM-Adopted</t>
   </si>
   <si>
     <t>Version</t>
@@ -36,13 +36,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>adopted</t>
+    <t>Adopted</t>
   </si>
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>adopted indication</t>
+    <t>Adopted indication</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-31T11:13:43-05:00</t>
+    <t>2022-04-11T07:37:02-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>When this family member is adopted.</t>
+    <t>When this family member is Adopted.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
convert to FHIR Core Profiles for vitalsigns, as are being forced now days.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-FM-adopted.xlsx
+++ b/docs/StructureDefinition-FM-adopted.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-12-06T12:46:33-06:00</t>
+    <t>2023-12-07T16:35:29-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,7 +129,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Element</t>
+    <t>element:FamilyMemberHistory</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>